<commit_message>
NB e MLP com Branch and Bound corrigidos
</commit_message>
<xml_diff>
--- a/atividade6-Naive Bayes/Branch and Bound/scores_balanced-Branch_and_Bound-Normalizado_SVC.xlsx
+++ b/atividade6-Naive Bayes/Branch and Bound/scores_balanced-Branch_and_Bound-Normalizado_SVC.xlsx
@@ -420,13 +420,13 @@
         <v>1</v>
       </c>
       <c r="D2">
-        <v>0.0847457627118644</v>
+        <v>0.5</v>
       </c>
       <c r="E2">
-        <v>1</v>
+        <v>0.4</v>
       </c>
       <c r="F2">
-        <v>0.3720930232558139</v>
+        <v>0.9418604651162791</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -440,13 +440,13 @@
         <v>2</v>
       </c>
       <c r="D3">
-        <v>0.03571428571428571</v>
+        <v>0.6666666666666666</v>
       </c>
       <c r="E3">
         <v>0.4</v>
       </c>
       <c r="F3">
-        <v>0.3372093023255814</v>
+        <v>0.9534883720930233</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -460,13 +460,13 @@
         <v>3</v>
       </c>
       <c r="D4">
-        <v>0.06896551724137931</v>
+        <v>0.6666666666666666</v>
       </c>
       <c r="E4">
         <v>0.8</v>
       </c>
       <c r="F4">
-        <v>0.3604651162790697</v>
+        <v>0.9651162790697675</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -480,13 +480,13 @@
         <v>4</v>
       </c>
       <c r="D5">
-        <v>0.09090909090909091</v>
+        <v>1</v>
       </c>
       <c r="E5">
-        <v>0.6666666666666666</v>
+        <v>0.8333333333333334</v>
       </c>
       <c r="F5">
-        <v>0.5116279069767442</v>
+        <v>0.9883720930232558</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -500,13 +500,13 @@
         <v>5</v>
       </c>
       <c r="D6">
-        <v>0.05882352941176471</v>
+        <v>0.2</v>
       </c>
       <c r="E6">
-        <v>0.3333333333333333</v>
+        <v>0.1666666666666667</v>
       </c>
       <c r="F6">
-        <v>0.5813953488372093</v>
+        <v>0.8953488372093024</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -520,13 +520,13 @@
         <v>6</v>
       </c>
       <c r="D7">
-        <v>0.15</v>
+        <v>1</v>
       </c>
       <c r="E7">
-        <v>0.5</v>
+        <v>0.6666666666666666</v>
       </c>
       <c r="F7">
-        <v>0.7674418604651163</v>
+        <v>0.9767441860465116</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -540,13 +540,13 @@
         <v>7</v>
       </c>
       <c r="D8">
-        <v>0.0625</v>
+        <v>1</v>
       </c>
       <c r="E8">
-        <v>0.3333333333333333</v>
+        <v>0.5</v>
       </c>
       <c r="F8">
-        <v>0.6046511627906976</v>
+        <v>0.9651162790697675</v>
       </c>
     </row>
     <row r="9" spans="1:6">
@@ -560,13 +560,13 @@
         <v>8</v>
       </c>
       <c r="D9">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="E9">
-        <v>0</v>
+        <v>0.1666666666666667</v>
       </c>
       <c r="F9">
-        <v>0.5465116279069767</v>
+        <v>0.9302325581395349</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -580,13 +580,13 @@
         <v>9</v>
       </c>
       <c r="D10">
-        <v>0.0625</v>
+        <v>1</v>
       </c>
       <c r="E10">
-        <v>0.6</v>
+        <v>0.2</v>
       </c>
       <c r="F10">
-        <v>0.4470588235294118</v>
+        <v>0.9529411764705882</v>
       </c>
     </row>
     <row r="11" spans="1:6">
@@ -600,13 +600,13 @@
         <v>10</v>
       </c>
       <c r="D11">
-        <v>0.06060606060606061</v>
+        <v>1</v>
       </c>
       <c r="E11">
         <v>0.4</v>
       </c>
       <c r="F11">
-        <v>0.6</v>
+        <v>0.9647058823529412</v>
       </c>
     </row>
     <row r="12" spans="1:6">
@@ -620,13 +620,13 @@
         <v>1</v>
       </c>
       <c r="D12">
-        <v>0.08196721311475409</v>
+        <v>0.5</v>
       </c>
       <c r="E12">
-        <v>1</v>
+        <v>0.4</v>
       </c>
       <c r="F12">
-        <v>0.3488372093023256</v>
+        <v>0.9418604651162791</v>
       </c>
     </row>
     <row r="13" spans="1:6">
@@ -640,13 +640,13 @@
         <v>2</v>
       </c>
       <c r="D13">
-        <v>0.03448275862068965</v>
+        <v>0.6666666666666666</v>
       </c>
       <c r="E13">
         <v>0.4</v>
       </c>
       <c r="F13">
-        <v>0.313953488372093</v>
+        <v>0.9534883720930233</v>
       </c>
     </row>
     <row r="14" spans="1:6">
@@ -660,13 +660,13 @@
         <v>3</v>
       </c>
       <c r="D14">
-        <v>0.06779661016949153</v>
+        <v>0.6666666666666666</v>
       </c>
       <c r="E14">
         <v>0.8</v>
       </c>
       <c r="F14">
-        <v>0.3488372093023256</v>
+        <v>0.9651162790697675</v>
       </c>
     </row>
     <row r="15" spans="1:6">
@@ -680,13 +680,13 @@
         <v>4</v>
       </c>
       <c r="D15">
-        <v>0.08888888888888889</v>
+        <v>1</v>
       </c>
       <c r="E15">
-        <v>0.6666666666666666</v>
+        <v>0.8333333333333334</v>
       </c>
       <c r="F15">
-        <v>0.5</v>
+        <v>0.9883720930232558</v>
       </c>
     </row>
     <row r="16" spans="1:6">
@@ -700,13 +700,13 @@
         <v>5</v>
       </c>
       <c r="D16">
-        <v>0.05882352941176471</v>
+        <v>0.2</v>
       </c>
       <c r="E16">
-        <v>0.3333333333333333</v>
+        <v>0.1666666666666667</v>
       </c>
       <c r="F16">
-        <v>0.5813953488372093</v>
+        <v>0.8953488372093024</v>
       </c>
     </row>
     <row r="17" spans="1:6">
@@ -720,13 +720,13 @@
         <v>6</v>
       </c>
       <c r="D17">
-        <v>0.15</v>
+        <v>1</v>
       </c>
       <c r="E17">
-        <v>0.5</v>
+        <v>0.6666666666666666</v>
       </c>
       <c r="F17">
-        <v>0.7674418604651163</v>
+        <v>0.9767441860465116</v>
       </c>
     </row>
     <row r="18" spans="1:6">
@@ -740,13 +740,13 @@
         <v>7</v>
       </c>
       <c r="D18">
-        <v>0.05882352941176471</v>
+        <v>1</v>
       </c>
       <c r="E18">
-        <v>0.3333333333333333</v>
+        <v>0.5</v>
       </c>
       <c r="F18">
-        <v>0.5813953488372093</v>
+        <v>0.9651162790697675</v>
       </c>
     </row>
     <row r="19" spans="1:6">
@@ -760,13 +760,13 @@
         <v>8</v>
       </c>
       <c r="D19">
-        <v>0.02631578947368421</v>
+        <v>0.5</v>
       </c>
       <c r="E19">
         <v>0.1666666666666667</v>
       </c>
       <c r="F19">
-        <v>0.5116279069767442</v>
+        <v>0.9302325581395349</v>
       </c>
     </row>
     <row r="20" spans="1:6">
@@ -780,13 +780,13 @@
         <v>9</v>
       </c>
       <c r="D20">
-        <v>0.06122448979591837</v>
+        <v>1</v>
       </c>
       <c r="E20">
-        <v>0.6</v>
+        <v>0.2</v>
       </c>
       <c r="F20">
-        <v>0.4352941176470588</v>
+        <v>0.9529411764705882</v>
       </c>
     </row>
     <row r="21" spans="1:6">
@@ -800,13 +800,13 @@
         <v>10</v>
       </c>
       <c r="D21">
-        <v>0.05714285714285714</v>
+        <v>1</v>
       </c>
       <c r="E21">
         <v>0.4</v>
       </c>
       <c r="F21">
-        <v>0.5764705882352941</v>
+        <v>0.9647058823529412</v>
       </c>
     </row>
     <row r="22" spans="1:6">
@@ -820,13 +820,13 @@
         <v>1</v>
       </c>
       <c r="D22">
-        <v>0.06557377049180328</v>
+        <v>0.5</v>
       </c>
       <c r="E22">
-        <v>0.8</v>
+        <v>0.4</v>
       </c>
       <c r="F22">
-        <v>0.3255813953488372</v>
+        <v>0.9418604651162791</v>
       </c>
     </row>
     <row r="23" spans="1:6">
@@ -840,13 +840,13 @@
         <v>2</v>
       </c>
       <c r="D23">
-        <v>0.03333333333333333</v>
+        <v>0.6666666666666666</v>
       </c>
       <c r="E23">
         <v>0.4</v>
       </c>
       <c r="F23">
-        <v>0.2906976744186047</v>
+        <v>0.9534883720930233</v>
       </c>
     </row>
     <row r="24" spans="1:6">
@@ -860,13 +860,13 @@
         <v>3</v>
       </c>
       <c r="D24">
-        <v>0.06779661016949153</v>
+        <v>0.6666666666666666</v>
       </c>
       <c r="E24">
         <v>0.8</v>
       </c>
       <c r="F24">
-        <v>0.3488372093023256</v>
+        <v>0.9651162790697675</v>
       </c>
     </row>
     <row r="25" spans="1:6">
@@ -880,13 +880,13 @@
         <v>4</v>
       </c>
       <c r="D25">
-        <v>0.08695652173913043</v>
+        <v>1</v>
       </c>
       <c r="E25">
-        <v>0.6666666666666666</v>
+        <v>0.8333333333333334</v>
       </c>
       <c r="F25">
-        <v>0.4883720930232558</v>
+        <v>0.9883720930232558</v>
       </c>
     </row>
     <row r="26" spans="1:6">
@@ -900,13 +900,13 @@
         <v>5</v>
       </c>
       <c r="D26">
-        <v>0.05555555555555555</v>
+        <v>0.2</v>
       </c>
       <c r="E26">
-        <v>0.3333333333333333</v>
+        <v>0.1666666666666667</v>
       </c>
       <c r="F26">
-        <v>0.5581395348837209</v>
+        <v>0.8953488372093024</v>
       </c>
     </row>
     <row r="27" spans="1:6">
@@ -920,13 +920,13 @@
         <v>6</v>
       </c>
       <c r="D27">
-        <v>0.15</v>
+        <v>1</v>
       </c>
       <c r="E27">
-        <v>0.5</v>
+        <v>0.6666666666666666</v>
       </c>
       <c r="F27">
-        <v>0.7674418604651163</v>
+        <v>0.9767441860465116</v>
       </c>
     </row>
     <row r="28" spans="1:6">
@@ -940,13 +940,13 @@
         <v>7</v>
       </c>
       <c r="D28">
-        <v>0.0625</v>
+        <v>1</v>
       </c>
       <c r="E28">
-        <v>0.3333333333333333</v>
+        <v>0.5</v>
       </c>
       <c r="F28">
-        <v>0.6046511627906976</v>
+        <v>0.9651162790697675</v>
       </c>
     </row>
     <row r="29" spans="1:6">
@@ -960,13 +960,13 @@
         <v>8</v>
       </c>
       <c r="D29">
-        <v>0.02564102564102564</v>
+        <v>0.5</v>
       </c>
       <c r="E29">
         <v>0.1666666666666667</v>
       </c>
       <c r="F29">
-        <v>0.5</v>
+        <v>0.9302325581395349</v>
       </c>
     </row>
     <row r="30" spans="1:6">
@@ -980,13 +980,13 @@
         <v>9</v>
       </c>
       <c r="D30">
-        <v>0.06</v>
+        <v>1</v>
       </c>
       <c r="E30">
-        <v>0.6</v>
+        <v>0.2</v>
       </c>
       <c r="F30">
-        <v>0.4235294117647059</v>
+        <v>0.9529411764705882</v>
       </c>
     </row>
     <row r="31" spans="1:6">
@@ -1000,13 +1000,13 @@
         <v>10</v>
       </c>
       <c r="D31">
-        <v>0.05405405405405406</v>
+        <v>1</v>
       </c>
       <c r="E31">
         <v>0.4</v>
       </c>
       <c r="F31">
-        <v>0.5529411764705883</v>
+        <v>0.9647058823529412</v>
       </c>
     </row>
     <row r="32" spans="1:6">
@@ -1020,13 +1020,13 @@
         <v>1</v>
       </c>
       <c r="D32">
-        <v>0.06451612903225806</v>
+        <v>0.5</v>
       </c>
       <c r="E32">
-        <v>0.8</v>
+        <v>0.4</v>
       </c>
       <c r="F32">
-        <v>0.313953488372093</v>
+        <v>0.9418604651162791</v>
       </c>
     </row>
     <row r="33" spans="1:6">
@@ -1040,13 +1040,13 @@
         <v>2</v>
       </c>
       <c r="D33">
-        <v>0.04761904761904762</v>
+        <v>0.6666666666666666</v>
       </c>
       <c r="E33">
-        <v>0.6</v>
+        <v>0.4</v>
       </c>
       <c r="F33">
-        <v>0.2790697674418605</v>
+        <v>0.9534883720930233</v>
       </c>
     </row>
     <row r="34" spans="1:6">
@@ -1060,13 +1060,13 @@
         <v>3</v>
       </c>
       <c r="D34">
-        <v>0.06779661016949153</v>
+        <v>0.6666666666666666</v>
       </c>
       <c r="E34">
         <v>0.8</v>
       </c>
       <c r="F34">
-        <v>0.3488372093023256</v>
+        <v>0.9651162790697675</v>
       </c>
     </row>
     <row r="35" spans="1:6">
@@ -1080,13 +1080,13 @@
         <v>4</v>
       </c>
       <c r="D35">
-        <v>0.08695652173913043</v>
+        <v>1</v>
       </c>
       <c r="E35">
-        <v>0.6666666666666666</v>
+        <v>0.8333333333333334</v>
       </c>
       <c r="F35">
-        <v>0.4883720930232558</v>
+        <v>0.9883720930232558</v>
       </c>
     </row>
     <row r="36" spans="1:6">
@@ -1100,13 +1100,13 @@
         <v>5</v>
       </c>
       <c r="D36">
-        <v>0.07894736842105263</v>
+        <v>0.2</v>
       </c>
       <c r="E36">
-        <v>0.5</v>
+        <v>0.1666666666666667</v>
       </c>
       <c r="F36">
-        <v>0.5581395348837209</v>
+        <v>0.8953488372093024</v>
       </c>
     </row>
     <row r="37" spans="1:6">
@@ -1120,13 +1120,13 @@
         <v>6</v>
       </c>
       <c r="D37">
-        <v>0.1176470588235294</v>
+        <v>1</v>
       </c>
       <c r="E37">
-        <v>0.3333333333333333</v>
+        <v>0.6666666666666666</v>
       </c>
       <c r="F37">
-        <v>0.7790697674418605</v>
+        <v>0.9767441860465116</v>
       </c>
     </row>
     <row r="38" spans="1:6">
@@ -1140,13 +1140,13 @@
         <v>7</v>
       </c>
       <c r="D38">
-        <v>0.0625</v>
+        <v>1</v>
       </c>
       <c r="E38">
-        <v>0.3333333333333333</v>
+        <v>0.5</v>
       </c>
       <c r="F38">
-        <v>0.6046511627906976</v>
+        <v>0.9651162790697675</v>
       </c>
     </row>
     <row r="39" spans="1:6">
@@ -1160,13 +1160,13 @@
         <v>8</v>
       </c>
       <c r="D39">
-        <v>0.025</v>
+        <v>0.5</v>
       </c>
       <c r="E39">
         <v>0.1666666666666667</v>
       </c>
       <c r="F39">
-        <v>0.4883720930232558</v>
+        <v>0.9302325581395349</v>
       </c>
     </row>
     <row r="40" spans="1:6">
@@ -1180,13 +1180,13 @@
         <v>9</v>
       </c>
       <c r="D40">
-        <v>0.06</v>
+        <v>1</v>
       </c>
       <c r="E40">
-        <v>0.6</v>
+        <v>0.2</v>
       </c>
       <c r="F40">
-        <v>0.4235294117647059</v>
+        <v>0.9529411764705882</v>
       </c>
     </row>
     <row r="41" spans="1:6">
@@ -1200,13 +1200,13 @@
         <v>10</v>
       </c>
       <c r="D41">
-        <v>0.05555555555555555</v>
+        <v>1</v>
       </c>
       <c r="E41">
         <v>0.4</v>
       </c>
       <c r="F41">
-        <v>0.5647058823529412</v>
+        <v>0.9647058823529412</v>
       </c>
     </row>
     <row r="42" spans="1:6">
@@ -1220,13 +1220,13 @@
         <v>1</v>
       </c>
       <c r="D42">
-        <v>0.0625</v>
+        <v>0.5</v>
       </c>
       <c r="E42">
-        <v>0.8</v>
+        <v>0.4</v>
       </c>
       <c r="F42">
-        <v>0.2906976744186047</v>
+        <v>0.9418604651162791</v>
       </c>
     </row>
     <row r="43" spans="1:6">
@@ -1240,13 +1240,13 @@
         <v>2</v>
       </c>
       <c r="D43">
-        <v>0.04761904761904762</v>
+        <v>0.6666666666666666</v>
       </c>
       <c r="E43">
-        <v>0.6</v>
+        <v>0.4</v>
       </c>
       <c r="F43">
-        <v>0.2790697674418605</v>
+        <v>0.9534883720930233</v>
       </c>
     </row>
     <row r="44" spans="1:6">
@@ -1260,13 +1260,13 @@
         <v>3</v>
       </c>
       <c r="D44">
-        <v>0.06779661016949153</v>
+        <v>0.6666666666666666</v>
       </c>
       <c r="E44">
         <v>0.8</v>
       </c>
       <c r="F44">
-        <v>0.3488372093023256</v>
+        <v>0.9651162790697675</v>
       </c>
     </row>
     <row r="45" spans="1:6">
@@ -1280,13 +1280,13 @@
         <v>4</v>
       </c>
       <c r="D45">
-        <v>0.06818181818181818</v>
+        <v>1</v>
       </c>
       <c r="E45">
-        <v>0.5</v>
+        <v>0.8333333333333334</v>
       </c>
       <c r="F45">
-        <v>0.4883720930232558</v>
+        <v>0.9883720930232558</v>
       </c>
     </row>
     <row r="46" spans="1:6">
@@ -1300,13 +1300,13 @@
         <v>5</v>
       </c>
       <c r="D46">
-        <v>0.07692307692307693</v>
+        <v>0.2</v>
       </c>
       <c r="E46">
-        <v>0.5</v>
+        <v>0.1666666666666667</v>
       </c>
       <c r="F46">
-        <v>0.5465116279069767</v>
+        <v>0.8953488372093024</v>
       </c>
     </row>
     <row r="47" spans="1:6">
@@ -1320,13 +1320,13 @@
         <v>6</v>
       </c>
       <c r="D47">
-        <v>0.125</v>
+        <v>1</v>
       </c>
       <c r="E47">
-        <v>0.3333333333333333</v>
+        <v>0.6666666666666666</v>
       </c>
       <c r="F47">
-        <v>0.7906976744186046</v>
+        <v>0.9767441860465116</v>
       </c>
     </row>
     <row r="48" spans="1:6">
@@ -1340,13 +1340,13 @@
         <v>7</v>
       </c>
       <c r="D48">
-        <v>0.06451612903225806</v>
+        <v>1</v>
       </c>
       <c r="E48">
-        <v>0.3333333333333333</v>
+        <v>0.5</v>
       </c>
       <c r="F48">
-        <v>0.6162790697674418</v>
+        <v>0.9651162790697675</v>
       </c>
     </row>
     <row r="49" spans="1:6">
@@ -1360,13 +1360,13 @@
         <v>8</v>
       </c>
       <c r="D49">
-        <v>0.02439024390243903</v>
+        <v>0.5</v>
       </c>
       <c r="E49">
         <v>0.1666666666666667</v>
       </c>
       <c r="F49">
-        <v>0.4767441860465116</v>
+        <v>0.9302325581395349</v>
       </c>
     </row>
     <row r="50" spans="1:6">
@@ -1380,13 +1380,13 @@
         <v>9</v>
       </c>
       <c r="D50">
-        <v>0.06</v>
+        <v>1</v>
       </c>
       <c r="E50">
-        <v>0.6</v>
+        <v>0.2</v>
       </c>
       <c r="F50">
-        <v>0.4235294117647059</v>
+        <v>0.9529411764705882</v>
       </c>
     </row>
     <row r="51" spans="1:6">
@@ -1400,13 +1400,13 @@
         <v>10</v>
       </c>
       <c r="D51">
-        <v>0.05714285714285714</v>
+        <v>1</v>
       </c>
       <c r="E51">
         <v>0.4</v>
       </c>
       <c r="F51">
-        <v>0.5764705882352941</v>
+        <v>0.9647058823529412</v>
       </c>
     </row>
     <row r="52" spans="1:6">
@@ -1420,13 +1420,13 @@
         <v>1</v>
       </c>
       <c r="D52">
-        <v>0.0625</v>
+        <v>0.5</v>
       </c>
       <c r="E52">
-        <v>0.8</v>
+        <v>0.4</v>
       </c>
       <c r="F52">
-        <v>0.2906976744186047</v>
+        <v>0.9418604651162791</v>
       </c>
     </row>
     <row r="53" spans="1:6">
@@ -1440,13 +1440,13 @@
         <v>2</v>
       </c>
       <c r="D53">
-        <v>0.04761904761904762</v>
+        <v>0.6666666666666666</v>
       </c>
       <c r="E53">
-        <v>0.6</v>
+        <v>0.4</v>
       </c>
       <c r="F53">
-        <v>0.2790697674418605</v>
+        <v>0.9534883720930233</v>
       </c>
     </row>
     <row r="54" spans="1:6">
@@ -1460,13 +1460,13 @@
         <v>3</v>
       </c>
       <c r="D54">
-        <v>0.06779661016949153</v>
+        <v>0.6666666666666666</v>
       </c>
       <c r="E54">
         <v>0.8</v>
       </c>
       <c r="F54">
-        <v>0.3488372093023256</v>
+        <v>0.9651162790697675</v>
       </c>
     </row>
     <row r="55" spans="1:6">
@@ -1480,13 +1480,13 @@
         <v>4</v>
       </c>
       <c r="D55">
-        <v>0.075</v>
+        <v>1</v>
       </c>
       <c r="E55">
-        <v>0.5</v>
+        <v>0.8333333333333334</v>
       </c>
       <c r="F55">
-        <v>0.5348837209302325</v>
+        <v>0.9883720930232558</v>
       </c>
     </row>
     <row r="56" spans="1:6">
@@ -1500,13 +1500,13 @@
         <v>5</v>
       </c>
       <c r="D56">
-        <v>0.07692307692307693</v>
+        <v>0.2</v>
       </c>
       <c r="E56">
-        <v>0.5</v>
+        <v>0.1666666666666667</v>
       </c>
       <c r="F56">
-        <v>0.5465116279069767</v>
+        <v>0.8953488372093024</v>
       </c>
     </row>
     <row r="57" spans="1:6">
@@ -1520,13 +1520,13 @@
         <v>6</v>
       </c>
       <c r="D57">
-        <v>0.1333333333333333</v>
+        <v>1</v>
       </c>
       <c r="E57">
-        <v>0.3333333333333333</v>
+        <v>0.6666666666666666</v>
       </c>
       <c r="F57">
-        <v>0.8023255813953488</v>
+        <v>0.9767441860465116</v>
       </c>
     </row>
     <row r="58" spans="1:6">
@@ -1540,13 +1540,13 @@
         <v>7</v>
       </c>
       <c r="D58">
-        <v>0.06666666666666667</v>
+        <v>1</v>
       </c>
       <c r="E58">
-        <v>0.3333333333333333</v>
+        <v>0.5</v>
       </c>
       <c r="F58">
-        <v>0.6279069767441861</v>
+        <v>0.9651162790697675</v>
       </c>
     </row>
     <row r="59" spans="1:6">
@@ -1560,13 +1560,13 @@
         <v>8</v>
       </c>
       <c r="D59">
-        <v>0.025</v>
+        <v>0.5</v>
       </c>
       <c r="E59">
         <v>0.1666666666666667</v>
       </c>
       <c r="F59">
-        <v>0.4883720930232558</v>
+        <v>0.9302325581395349</v>
       </c>
     </row>
     <row r="60" spans="1:6">
@@ -1580,13 +1580,13 @@
         <v>9</v>
       </c>
       <c r="D60">
-        <v>0.05882352941176471</v>
+        <v>1</v>
       </c>
       <c r="E60">
-        <v>0.6</v>
+        <v>0.2</v>
       </c>
       <c r="F60">
-        <v>0.4117647058823529</v>
+        <v>0.9529411764705882</v>
       </c>
     </row>
     <row r="61" spans="1:6">
@@ -1600,13 +1600,13 @@
         <v>10</v>
       </c>
       <c r="D61">
-        <v>0.05714285714285714</v>
+        <v>1</v>
       </c>
       <c r="E61">
         <v>0.4</v>
       </c>
       <c r="F61">
-        <v>0.5764705882352941</v>
+        <v>0.9647058823529412</v>
       </c>
     </row>
     <row r="62" spans="1:6">
@@ -1620,13 +1620,13 @@
         <v>1</v>
       </c>
       <c r="D62">
-        <v>0.06153846153846154</v>
+        <v>0.5</v>
       </c>
       <c r="E62">
-        <v>0.8</v>
+        <v>0.4</v>
       </c>
       <c r="F62">
-        <v>0.2790697674418605</v>
+        <v>0.9418604651162791</v>
       </c>
     </row>
     <row r="63" spans="1:6">
@@ -1640,13 +1640,13 @@
         <v>2</v>
       </c>
       <c r="D63">
-        <v>0.04615384615384616</v>
+        <v>0.6666666666666666</v>
       </c>
       <c r="E63">
-        <v>0.6</v>
+        <v>0.4</v>
       </c>
       <c r="F63">
-        <v>0.2558139534883721</v>
+        <v>0.9534883720930233</v>
       </c>
     </row>
     <row r="64" spans="1:6">
@@ -1660,13 +1660,13 @@
         <v>3</v>
       </c>
       <c r="D64">
-        <v>0.06779661016949153</v>
+        <v>0.6666666666666666</v>
       </c>
       <c r="E64">
         <v>0.8</v>
       </c>
       <c r="F64">
-        <v>0.3488372093023256</v>
+        <v>0.9651162790697675</v>
       </c>
     </row>
     <row r="65" spans="1:6">
@@ -1680,13 +1680,13 @@
         <v>4</v>
       </c>
       <c r="D65">
-        <v>0.08333333333333333</v>
+        <v>1</v>
       </c>
       <c r="E65">
-        <v>0.5</v>
+        <v>0.8333333333333334</v>
       </c>
       <c r="F65">
-        <v>0.5813953488372093</v>
+        <v>0.9883720930232558</v>
       </c>
     </row>
     <row r="66" spans="1:6">
@@ -1700,13 +1700,13 @@
         <v>5</v>
       </c>
       <c r="D66">
-        <v>0.07894736842105263</v>
+        <v>0.2</v>
       </c>
       <c r="E66">
-        <v>0.5</v>
+        <v>0.1666666666666667</v>
       </c>
       <c r="F66">
-        <v>0.5581395348837209</v>
+        <v>0.8953488372093024</v>
       </c>
     </row>
     <row r="67" spans="1:6">
@@ -1720,13 +1720,13 @@
         <v>6</v>
       </c>
       <c r="D67">
-        <v>0.1333333333333333</v>
+        <v>1</v>
       </c>
       <c r="E67">
-        <v>0.3333333333333333</v>
+        <v>0.6666666666666666</v>
       </c>
       <c r="F67">
-        <v>0.8023255813953488</v>
+        <v>0.9767441860465116</v>
       </c>
     </row>
     <row r="68" spans="1:6">
@@ -1740,13 +1740,13 @@
         <v>7</v>
       </c>
       <c r="D68">
-        <v>0.06666666666666667</v>
+        <v>1</v>
       </c>
       <c r="E68">
-        <v>0.3333333333333333</v>
+        <v>0.5</v>
       </c>
       <c r="F68">
-        <v>0.6279069767441861</v>
+        <v>0.9651162790697675</v>
       </c>
     </row>
     <row r="69" spans="1:6">
@@ -1760,13 +1760,13 @@
         <v>8</v>
       </c>
       <c r="D69">
-        <v>0.025</v>
+        <v>0.5</v>
       </c>
       <c r="E69">
         <v>0.1666666666666667</v>
       </c>
       <c r="F69">
-        <v>0.4883720930232558</v>
+        <v>0.9302325581395349</v>
       </c>
     </row>
     <row r="70" spans="1:6">
@@ -1780,13 +1780,13 @@
         <v>9</v>
       </c>
       <c r="D70">
-        <v>0.05882352941176471</v>
+        <v>1</v>
       </c>
       <c r="E70">
-        <v>0.6</v>
+        <v>0.2</v>
       </c>
       <c r="F70">
-        <v>0.4117647058823529</v>
+        <v>0.9529411764705882</v>
       </c>
     </row>
     <row r="71" spans="1:6">
@@ -1800,13 +1800,13 @@
         <v>10</v>
       </c>
       <c r="D71">
-        <v>0.05882352941176471</v>
+        <v>1</v>
       </c>
       <c r="E71">
         <v>0.4</v>
       </c>
       <c r="F71">
-        <v>0.5882352941176471</v>
+        <v>0.9647058823529412</v>
       </c>
     </row>
     <row r="72" spans="1:6">
@@ -1820,13 +1820,13 @@
         <v>1</v>
       </c>
       <c r="D72">
-        <v>0.06060606060606061</v>
+        <v>0.5</v>
       </c>
       <c r="E72">
-        <v>0.8</v>
+        <v>0.4</v>
       </c>
       <c r="F72">
-        <v>0.2674418604651163</v>
+        <v>0.9418604651162791</v>
       </c>
     </row>
     <row r="73" spans="1:6">
@@ -1840,13 +1840,13 @@
         <v>2</v>
       </c>
       <c r="D73">
-        <v>0.04347826086956522</v>
+        <v>0.6666666666666666</v>
       </c>
       <c r="E73">
-        <v>0.6</v>
+        <v>0.4</v>
       </c>
       <c r="F73">
-        <v>0.2093023255813954</v>
+        <v>0.9534883720930233</v>
       </c>
     </row>
     <row r="74" spans="1:6">
@@ -1860,13 +1860,13 @@
         <v>3</v>
       </c>
       <c r="D74">
-        <v>0.06896551724137931</v>
+        <v>0.6666666666666666</v>
       </c>
       <c r="E74">
         <v>0.8</v>
       </c>
       <c r="F74">
-        <v>0.3604651162790697</v>
+        <v>0.9651162790697675</v>
       </c>
     </row>
     <row r="75" spans="1:6">
@@ -1880,13 +1880,13 @@
         <v>4</v>
       </c>
       <c r="D75">
-        <v>0.08333333333333333</v>
+        <v>1</v>
       </c>
       <c r="E75">
-        <v>0.5</v>
+        <v>0.8333333333333334</v>
       </c>
       <c r="F75">
-        <v>0.5813953488372093</v>
+        <v>0.9883720930232558</v>
       </c>
     </row>
     <row r="76" spans="1:6">
@@ -1900,13 +1900,13 @@
         <v>5</v>
       </c>
       <c r="D76">
-        <v>0.07894736842105263</v>
+        <v>0.2</v>
       </c>
       <c r="E76">
-        <v>0.5</v>
+        <v>0.1666666666666667</v>
       </c>
       <c r="F76">
-        <v>0.5581395348837209</v>
+        <v>0.8953488372093024</v>
       </c>
     </row>
     <row r="77" spans="1:6">
@@ -1920,13 +1920,13 @@
         <v>6</v>
       </c>
       <c r="D77">
-        <v>0.1333333333333333</v>
+        <v>1</v>
       </c>
       <c r="E77">
-        <v>0.3333333333333333</v>
+        <v>0.6666666666666666</v>
       </c>
       <c r="F77">
-        <v>0.8023255813953488</v>
+        <v>0.9767441860465116</v>
       </c>
     </row>
     <row r="78" spans="1:6">
@@ -1940,13 +1940,13 @@
         <v>7</v>
       </c>
       <c r="D78">
-        <v>0.06666666666666667</v>
+        <v>1</v>
       </c>
       <c r="E78">
-        <v>0.3333333333333333</v>
+        <v>0.5</v>
       </c>
       <c r="F78">
-        <v>0.6279069767441861</v>
+        <v>0.9651162790697675</v>
       </c>
     </row>
     <row r="79" spans="1:6">
@@ -1960,13 +1960,13 @@
         <v>8</v>
       </c>
       <c r="D79">
-        <v>0.02564102564102564</v>
+        <v>0.5</v>
       </c>
       <c r="E79">
         <v>0.1666666666666667</v>
       </c>
       <c r="F79">
-        <v>0.5</v>
+        <v>0.9302325581395349</v>
       </c>
     </row>
     <row r="80" spans="1:6">
@@ -1980,13 +1980,13 @@
         <v>9</v>
       </c>
       <c r="D80">
-        <v>0.05882352941176471</v>
+        <v>1</v>
       </c>
       <c r="E80">
-        <v>0.6</v>
+        <v>0.2</v>
       </c>
       <c r="F80">
-        <v>0.4117647058823529</v>
+        <v>0.9529411764705882</v>
       </c>
     </row>
     <row r="81" spans="1:6">
@@ -2000,13 +2000,13 @@
         <v>10</v>
       </c>
       <c r="D81">
-        <v>0.06060606060606061</v>
+        <v>1</v>
       </c>
       <c r="E81">
         <v>0.4</v>
       </c>
       <c r="F81">
-        <v>0.6</v>
+        <v>0.9647058823529412</v>
       </c>
     </row>
     <row r="82" spans="1:6">
@@ -2020,13 +2020,13 @@
         <v>1</v>
       </c>
       <c r="D82">
-        <v>0.06060606060606061</v>
+        <v>0.5</v>
       </c>
       <c r="E82">
-        <v>0.8</v>
+        <v>0.4</v>
       </c>
       <c r="F82">
-        <v>0.2674418604651163</v>
+        <v>0.9418604651162791</v>
       </c>
     </row>
     <row r="83" spans="1:6">
@@ -2040,13 +2040,13 @@
         <v>2</v>
       </c>
       <c r="D83">
-        <v>0.04347826086956522</v>
+        <v>0.6666666666666666</v>
       </c>
       <c r="E83">
-        <v>0.6</v>
+        <v>0.4</v>
       </c>
       <c r="F83">
-        <v>0.2093023255813954</v>
+        <v>0.9534883720930233</v>
       </c>
     </row>
     <row r="84" spans="1:6">
@@ -2060,13 +2060,13 @@
         <v>3</v>
       </c>
       <c r="D84">
-        <v>0.06896551724137931</v>
+        <v>0.6666666666666666</v>
       </c>
       <c r="E84">
         <v>0.8</v>
       </c>
       <c r="F84">
-        <v>0.3604651162790697</v>
+        <v>0.9651162790697675</v>
       </c>
     </row>
     <row r="85" spans="1:6">
@@ -2080,13 +2080,13 @@
         <v>4</v>
       </c>
       <c r="D85">
-        <v>0.08823529411764706</v>
+        <v>1</v>
       </c>
       <c r="E85">
-        <v>0.5</v>
+        <v>0.8333333333333334</v>
       </c>
       <c r="F85">
-        <v>0.6046511627906976</v>
+        <v>0.9883720930232558</v>
       </c>
     </row>
     <row r="86" spans="1:6">
@@ -2100,13 +2100,13 @@
         <v>5</v>
       </c>
       <c r="D86">
-        <v>0.07894736842105263</v>
+        <v>0.2</v>
       </c>
       <c r="E86">
-        <v>0.5</v>
+        <v>0.1666666666666667</v>
       </c>
       <c r="F86">
-        <v>0.5581395348837209</v>
+        <v>0.8953488372093024</v>
       </c>
     </row>
     <row r="87" spans="1:6">
@@ -2120,13 +2120,13 @@
         <v>6</v>
       </c>
       <c r="D87">
-        <v>0.1333333333333333</v>
+        <v>1</v>
       </c>
       <c r="E87">
-        <v>0.3333333333333333</v>
+        <v>0.6666666666666666</v>
       </c>
       <c r="F87">
-        <v>0.8023255813953488</v>
+        <v>0.9767441860465116</v>
       </c>
     </row>
     <row r="88" spans="1:6">
@@ -2140,13 +2140,13 @@
         <v>7</v>
       </c>
       <c r="D88">
-        <v>0.06896551724137931</v>
+        <v>1</v>
       </c>
       <c r="E88">
-        <v>0.3333333333333333</v>
+        <v>0.5</v>
       </c>
       <c r="F88">
-        <v>0.6395348837209303</v>
+        <v>0.9651162790697675</v>
       </c>
     </row>
     <row r="89" spans="1:6">
@@ -2160,13 +2160,13 @@
         <v>8</v>
       </c>
       <c r="D89">
-        <v>0.02777777777777778</v>
+        <v>0.5</v>
       </c>
       <c r="E89">
         <v>0.1666666666666667</v>
       </c>
       <c r="F89">
-        <v>0.5348837209302325</v>
+        <v>0.9302325581395349</v>
       </c>
     </row>
     <row r="90" spans="1:6">
@@ -2180,13 +2180,13 @@
         <v>9</v>
       </c>
       <c r="D90">
-        <v>0.05882352941176471</v>
+        <v>1</v>
       </c>
       <c r="E90">
-        <v>0.6</v>
+        <v>0.2</v>
       </c>
       <c r="F90">
-        <v>0.4117647058823529</v>
+        <v>0.9529411764705882</v>
       </c>
     </row>
     <row r="91" spans="1:6">
@@ -2200,13 +2200,13 @@
         <v>10</v>
       </c>
       <c r="D91">
-        <v>0.06060606060606061</v>
+        <v>1</v>
       </c>
       <c r="E91">
         <v>0.4</v>
       </c>
       <c r="F91">
-        <v>0.6</v>
+        <v>0.9647058823529412</v>
       </c>
     </row>
     <row r="92" spans="1:6">
@@ -2220,13 +2220,13 @@
         <v>1</v>
       </c>
       <c r="D92">
-        <v>0.05882352941176471</v>
+        <v>0.5</v>
       </c>
       <c r="E92">
-        <v>0.8</v>
+        <v>0.4</v>
       </c>
       <c r="F92">
-        <v>0.2441860465116279</v>
+        <v>0.9418604651162791</v>
       </c>
     </row>
     <row r="93" spans="1:6">
@@ -2240,13 +2240,13 @@
         <v>2</v>
       </c>
       <c r="D93">
-        <v>0.04285714285714286</v>
+        <v>0.6666666666666666</v>
       </c>
       <c r="E93">
-        <v>0.6</v>
+        <v>0.4</v>
       </c>
       <c r="F93">
-        <v>0.1976744186046512</v>
+        <v>0.9534883720930233</v>
       </c>
     </row>
     <row r="94" spans="1:6">
@@ -2260,13 +2260,13 @@
         <v>3</v>
       </c>
       <c r="D94">
-        <v>0.07017543859649122</v>
+        <v>0.6666666666666666</v>
       </c>
       <c r="E94">
         <v>0.8</v>
       </c>
       <c r="F94">
-        <v>0.3720930232558139</v>
+        <v>0.9651162790697675</v>
       </c>
     </row>
     <row r="95" spans="1:6">
@@ -2280,13 +2280,13 @@
         <v>4</v>
       </c>
       <c r="D95">
-        <v>0.08823529411764706</v>
+        <v>1</v>
       </c>
       <c r="E95">
-        <v>0.5</v>
+        <v>0.8333333333333334</v>
       </c>
       <c r="F95">
-        <v>0.6046511627906976</v>
+        <v>0.9883720930232558</v>
       </c>
     </row>
     <row r="96" spans="1:6">
@@ -2300,13 +2300,13 @@
         <v>5</v>
       </c>
       <c r="D96">
-        <v>0.08108108108108109</v>
+        <v>0.2</v>
       </c>
       <c r="E96">
-        <v>0.5</v>
+        <v>0.1666666666666667</v>
       </c>
       <c r="F96">
-        <v>0.5697674418604651</v>
+        <v>0.8953488372093024</v>
       </c>
     </row>
     <row r="97" spans="1:6">
@@ -2320,13 +2320,13 @@
         <v>6</v>
       </c>
       <c r="D97">
-        <v>0.125</v>
+        <v>1</v>
       </c>
       <c r="E97">
-        <v>0.3333333333333333</v>
+        <v>0.6666666666666666</v>
       </c>
       <c r="F97">
-        <v>0.7906976744186046</v>
+        <v>0.9767441860465116</v>
       </c>
     </row>
     <row r="98" spans="1:6">
@@ -2340,13 +2340,13 @@
         <v>7</v>
       </c>
       <c r="D98">
-        <v>0.06896551724137931</v>
+        <v>1</v>
       </c>
       <c r="E98">
-        <v>0.3333333333333333</v>
+        <v>0.5</v>
       </c>
       <c r="F98">
-        <v>0.6395348837209303</v>
+        <v>0.9651162790697675</v>
       </c>
     </row>
     <row r="99" spans="1:6">
@@ -2360,13 +2360,13 @@
         <v>8</v>
       </c>
       <c r="D99">
-        <v>0.02777777777777778</v>
+        <v>0.5</v>
       </c>
       <c r="E99">
         <v>0.1666666666666667</v>
       </c>
       <c r="F99">
-        <v>0.5348837209302325</v>
+        <v>0.9302325581395349</v>
       </c>
     </row>
     <row r="100" spans="1:6">
@@ -2380,13 +2380,13 @@
         <v>9</v>
       </c>
       <c r="D100">
-        <v>0.05882352941176471</v>
+        <v>1</v>
       </c>
       <c r="E100">
-        <v>0.6</v>
+        <v>0.2</v>
       </c>
       <c r="F100">
-        <v>0.4117647058823529</v>
+        <v>0.9529411764705882</v>
       </c>
     </row>
     <row r="101" spans="1:6">
@@ -2400,13 +2400,13 @@
         <v>10</v>
       </c>
       <c r="D101">
-        <v>0.06666666666666667</v>
+        <v>1</v>
       </c>
       <c r="E101">
         <v>0.4</v>
       </c>
       <c r="F101">
-        <v>0.6352941176470588</v>
+        <v>0.9647058823529412</v>
       </c>
     </row>
   </sheetData>

</xml_diff>